<commit_message>
route_of_admin & product_type fixes.
</commit_message>
<xml_diff>
--- a/static/fields/animalandveterinarylabel_reference.xlsx
+++ b/static/fields/animalandveterinarylabel_reference.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackfinch/WebstormProjects/open.fda.gov/static/fields/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack.finch/WebstormProjects/open.fda.gov/static/fields/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF30E1D6-E54D-8146-8326-85F0425B4EB0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19AEA3D7-4F8C-2B46-8B49-23DE97B83F60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="218">
   <si>
     <t>Field Name</t>
   </si>
@@ -676,6 +676,9 @@
   </si>
   <si>
     <t>Information about side effects that people may experience, and the substances (e.g. alcohol) or activities (e.g. operating machinery, driving a car) to avoid while using the drug product.</t>
+  </si>
+  <si>
+    <t>route_of_administration</t>
   </si>
 </sst>
 </file>
@@ -1304,8 +1307,8 @@
   </sheetPr>
   <dimension ref="A1:E110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="C111" sqref="C111:E122"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1644,7 +1647,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:5" ht="34" x14ac:dyDescent="0.2">
       <c r="B26" s="4" t="s">
         <v>55</v>
       </c>
@@ -1830,7 +1833,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:5" ht="51" x14ac:dyDescent="0.2">
       <c r="B41" s="4" t="s">
         <v>83</v>
       </c>
@@ -1911,7 +1914,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:5" ht="51" x14ac:dyDescent="0.2">
       <c r="B47" s="4" t="s">
         <v>96</v>
       </c>
@@ -1925,7 +1928,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="48" spans="2:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:5" ht="51" x14ac:dyDescent="0.2">
       <c r="B48" s="4" t="s">
         <v>97</v>
       </c>
@@ -1939,7 +1942,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="B49" s="4" t="s">
         <v>100</v>
       </c>
@@ -1981,7 +1984,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="B52" s="4" t="s">
         <v>104</v>
       </c>
@@ -2107,7 +2110,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>109</v>
       </c>
@@ -2135,7 +2138,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>109</v>
       </c>
@@ -2149,7 +2152,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>109</v>
       </c>
@@ -2261,7 +2264,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>109</v>
       </c>
@@ -2317,7 +2320,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="B76" s="4" t="s">
         <v>156</v>
       </c>
@@ -2359,7 +2362,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="B79" s="4" t="s">
         <v>163</v>
       </c>
@@ -2440,7 +2443,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B85" s="4" t="s">
         <v>171</v>
       </c>
@@ -2468,7 +2471,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:5" ht="51" x14ac:dyDescent="0.2">
       <c r="B87" s="4" t="s">
         <v>175</v>
       </c>
@@ -2507,7 +2510,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B90" s="4" t="s">
         <v>180</v>
       </c>
@@ -2518,18 +2521,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B91" s="4" t="s">
-        <v>136</v>
+        <v>217</v>
       </c>
       <c r="C91" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B92" s="4" t="s">
         <v>181</v>
       </c>
@@ -2776,8 +2779,9 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="21" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="33" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>